<commit_message>
updated colors for street needs
</commit_message>
<xml_diff>
--- a/underlying_data/toronto-shelter-system-flow_april27.xlsx
+++ b/underlying_data/toronto-shelter-system-flow_april27.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/merenberg/Desktop/dash-project/underlying_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7E2598DC-89D3-D74D-A673-1E7E78F5AD05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995AAE94-89BA-D04D-8D35-4741B877FD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="480" windowWidth="28800" windowHeight="16240"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="toronto-shelter-system-flow_apr" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'toronto-shelter-system-flow_apr'!$A$1:$R$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'toronto-shelter-system-flow_apr'!$A$1:$R$106</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -949,11 +949,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:R106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1070,7 +1071,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>100</v>
       </c>
@@ -1126,7 +1127,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>101</v>
       </c>
@@ -1182,7 +1183,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>102</v>
       </c>
@@ -1238,7 +1239,7 @@
         <v>27.3</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>103</v>
       </c>
@@ -1294,7 +1295,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>104</v>
       </c>
@@ -1350,7 +1351,7 @@
         <v>62.8</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>105</v>
       </c>
@@ -1462,7 +1463,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>107</v>
       </c>
@@ -1518,7 +1519,7 @@
         <v>34.700000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>108</v>
       </c>
@@ -1574,7 +1575,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>109</v>
       </c>
@@ -1630,7 +1631,7 @@
         <v>27.3</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>110</v>
       </c>
@@ -1686,7 +1687,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>111</v>
       </c>
@@ -1742,7 +1743,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>112</v>
       </c>
@@ -1854,7 +1855,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>114</v>
       </c>
@@ -1910,7 +1911,7 @@
         <v>35.799999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>115</v>
       </c>
@@ -1966,7 +1967,7 @@
         <v>28.8</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>116</v>
       </c>
@@ -2022,7 +2023,7 @@
         <v>27.2</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>117</v>
       </c>
@@ -2078,7 +2079,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>118</v>
       </c>
@@ -2134,7 +2135,7 @@
         <v>63.4</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>119</v>
       </c>
@@ -2246,7 +2247,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>121</v>
       </c>
@@ -2302,7 +2303,7 @@
         <v>43.1</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>122</v>
       </c>
@@ -2358,7 +2359,7 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>123</v>
       </c>
@@ -2414,7 +2415,7 @@
         <v>31.2</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>124</v>
       </c>
@@ -2470,7 +2471,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>125</v>
       </c>
@@ -2526,7 +2527,7 @@
         <v>58.5</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>126</v>
       </c>
@@ -2638,7 +2639,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>128</v>
       </c>
@@ -2694,7 +2695,7 @@
         <v>43.2</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>129</v>
       </c>
@@ -2750,7 +2751,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>130</v>
       </c>
@@ -2806,7 +2807,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>131</v>
       </c>
@@ -2862,7 +2863,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>132</v>
       </c>
@@ -2918,7 +2919,7 @@
         <v>63.6</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>133</v>
       </c>
@@ -3030,7 +3031,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>135</v>
       </c>
@@ -3086,7 +3087,7 @@
         <v>47.1</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>136</v>
       </c>
@@ -3142,7 +3143,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>137</v>
       </c>
@@ -3198,7 +3199,7 @@
         <v>27.2</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>138</v>
       </c>
@@ -3254,7 +3255,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>139</v>
       </c>
@@ -3310,7 +3311,7 @@
         <v>63.6</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>140</v>
       </c>
@@ -3422,7 +3423,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>142</v>
       </c>
@@ -3478,7 +3479,7 @@
         <v>47.6</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>143</v>
       </c>
@@ -3534,7 +3535,7 @@
         <v>21.8</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>144</v>
       </c>
@@ -3590,7 +3591,7 @@
         <v>25.8</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>145</v>
       </c>
@@ -3646,7 +3647,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>146</v>
       </c>
@@ -3702,7 +3703,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>147</v>
       </c>
@@ -3814,7 +3815,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>149</v>
       </c>
@@ -3870,7 +3871,7 @@
         <v>50.6</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>150</v>
       </c>
@@ -3926,7 +3927,7 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>151</v>
       </c>
@@ -3982,7 +3983,7 @@
         <v>24.8</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>152</v>
       </c>
@@ -4038,7 +4039,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>153</v>
       </c>
@@ -4094,7 +4095,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>154</v>
       </c>
@@ -4206,7 +4207,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>156</v>
       </c>
@@ -4262,7 +4263,7 @@
         <v>49.9</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>157</v>
       </c>
@@ -4318,7 +4319,7 @@
         <v>18.7</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>158</v>
       </c>
@@ -4374,7 +4375,7 @@
         <v>21.3</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>159</v>
       </c>
@@ -4430,7 +4431,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>160</v>
       </c>
@@ -4486,7 +4487,7 @@
         <v>69.3</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>161</v>
       </c>
@@ -4598,7 +4599,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>163</v>
       </c>
@@ -4654,7 +4655,7 @@
         <v>49.2</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>164</v>
       </c>
@@ -4710,7 +4711,7 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>165</v>
       </c>
@@ -4766,7 +4767,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>166</v>
       </c>
@@ -4822,7 +4823,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>167</v>
       </c>
@@ -4878,7 +4879,7 @@
         <v>70.900000000000006</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>168</v>
       </c>
@@ -4990,7 +4991,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>170</v>
       </c>
@@ -5046,7 +5047,7 @@
         <v>46.8</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>171</v>
       </c>
@@ -5102,7 +5103,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>172</v>
       </c>
@@ -5158,7 +5159,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>173</v>
       </c>
@@ -5214,7 +5215,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>174</v>
       </c>
@@ -5270,7 +5271,7 @@
         <v>72.7</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>175</v>
       </c>
@@ -5382,7 +5383,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>177</v>
       </c>
@@ -5438,7 +5439,7 @@
         <v>45.6</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>178</v>
       </c>
@@ -5494,7 +5495,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>179</v>
       </c>
@@ -5550,7 +5551,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>180</v>
       </c>
@@ -5606,7 +5607,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>181</v>
       </c>
@@ -5662,7 +5663,7 @@
         <v>73.900000000000006</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>182</v>
       </c>
@@ -5774,7 +5775,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>184</v>
       </c>
@@ -5830,7 +5831,7 @@
         <v>45.3</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>185</v>
       </c>
@@ -5886,7 +5887,7 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>186</v>
       </c>
@@ -5942,7 +5943,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>187</v>
       </c>
@@ -5998,7 +5999,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>188</v>
       </c>
@@ -6054,7 +6055,7 @@
         <v>74.599999999999994</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>189</v>
       </c>
@@ -6166,7 +6167,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>191</v>
       </c>
@@ -6222,7 +6223,7 @@
         <v>45.8</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>192</v>
       </c>
@@ -6278,7 +6279,7 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>193</v>
       </c>
@@ -6334,7 +6335,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>194</v>
       </c>
@@ -6390,7 +6391,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>195</v>
       </c>
@@ -6446,7 +6447,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>196</v>
       </c>
@@ -6558,7 +6559,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>198</v>
       </c>
@@ -6614,7 +6615,7 @@
         <v>46.7</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>199</v>
       </c>
@@ -6670,7 +6671,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>200</v>
       </c>
@@ -6726,7 +6727,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>201</v>
       </c>
@@ -6782,7 +6783,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>202</v>
       </c>
@@ -6838,7 +6839,7 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>203</v>
       </c>
@@ -6895,7 +6896,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R1"/>
+  <autoFilter ref="A1:R106" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="All Population"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>